<commit_message>
update screenshot for the password
</commit_message>
<xml_diff>
--- a/win10+lan.xlsx
+++ b/win10+lan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mpsuzuki\Documents\2021_03\初期講習会\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C68488DA-3141-4F48-BA8A-71F61FB45112}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{690C1B87-F5E5-4DF9-A88B-709ED26B4B39}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="15468" windowHeight="6396" tabRatio="782" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6210,8 +6210,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:XFD18"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>

</xml_diff>